<commit_message>
Updated Database_Thresholds indicator quantile files.
</commit_message>
<xml_diff>
--- a/output/ScriptResults/Database_Thresholds.xlsx
+++ b/output/ScriptResults/Database_Thresholds.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="287">
   <si>
     <t>ThresholdID</t>
   </si>
@@ -876,6 +876,12 @@
   </si>
   <si>
     <t xml:space="preserve">Calculated Total Nitrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IndicatorQuantiles.R, Git Commit ID: db49f0f869e1f5a8558dc746458075a467cf2c41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database_Thresholds_details.xlsx, Git Commit ID: 17b6a0f858dccbb28fc8ab3fe179e7fa731e5996</t>
   </si>
 </sst>
 </file>
@@ -897,8 +903,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
       <b/>
       <i/>
     </font>
@@ -906,24 +910,18 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
       <b/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
       <i/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1473,7 +1471,7 @@
       <c r="U4"/>
       <c r="V4"/>
       <c r="W4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X4" s="5" t="n">
         <v>45299</v>
@@ -1536,7 +1534,7 @@
       </c>
       <c r="V5"/>
       <c r="W5" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X5" s="5" t="n">
         <v>45299</v>
@@ -1597,7 +1595,7 @@
       </c>
       <c r="V6"/>
       <c r="W6" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X6" s="5" t="n">
         <v>45299</v>
@@ -1656,7 +1654,7 @@
       </c>
       <c r="V7"/>
       <c r="W7" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X7" s="5" t="n">
         <v>45299</v>
@@ -1707,7 +1705,7 @@
       <c r="U8"/>
       <c r="V8"/>
       <c r="W8" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X8" s="5" t="n">
         <v>45299</v>
@@ -1768,7 +1766,7 @@
       </c>
       <c r="V9"/>
       <c r="W9" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X9" s="5" t="n">
         <v>45299</v>
@@ -1827,7 +1825,7 @@
       </c>
       <c r="V10"/>
       <c r="W10" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X10" s="5" t="n">
         <v>45299</v>
@@ -1886,7 +1884,7 @@
       </c>
       <c r="V11"/>
       <c r="W11" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X11" s="5" t="n">
         <v>45299</v>
@@ -1947,7 +1945,7 @@
       </c>
       <c r="V12"/>
       <c r="W12" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X12" s="5" t="n">
         <v>45299</v>
@@ -2004,7 +2002,7 @@
       <c r="U13"/>
       <c r="V13"/>
       <c r="W13" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X13" s="5" t="n">
         <v>45299</v>
@@ -2063,7 +2061,7 @@
       </c>
       <c r="V14"/>
       <c r="W14" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X14" s="5" t="n">
         <v>45299</v>
@@ -2124,7 +2122,7 @@
       </c>
       <c r="V15"/>
       <c r="W15" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X15" s="5" t="n">
         <v>45299</v>
@@ -2185,7 +2183,7 @@
       </c>
       <c r="V16"/>
       <c r="W16" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X16" s="5" t="n">
         <v>45299</v>
@@ -2246,7 +2244,7 @@
       </c>
       <c r="V17"/>
       <c r="W17" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X17" s="5" t="n">
         <v>45299</v>
@@ -2307,7 +2305,7 @@
       </c>
       <c r="V18"/>
       <c r="W18" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X18" s="5" t="n">
         <v>45299</v>
@@ -2370,7 +2368,7 @@
       </c>
       <c r="V19"/>
       <c r="W19" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X19" s="5" t="n">
         <v>45299</v>
@@ -2429,7 +2427,7 @@
       </c>
       <c r="V20"/>
       <c r="W20" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X20" s="5" t="n">
         <v>45299</v>
@@ -2480,7 +2478,7 @@
       <c r="U21"/>
       <c r="V21"/>
       <c r="W21" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X21" s="5" t="n">
         <v>45299</v>
@@ -2537,7 +2535,7 @@
       </c>
       <c r="V22"/>
       <c r="W22" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X22" s="5" t="n">
         <v>45299</v>
@@ -2600,7 +2598,7 @@
       </c>
       <c r="V23"/>
       <c r="W23" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X23" s="5" t="n">
         <v>45299</v>
@@ -2665,7 +2663,7 @@
       </c>
       <c r="V24"/>
       <c r="W24" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X24" s="5" t="n">
         <v>45299</v>
@@ -2730,7 +2728,7 @@
       </c>
       <c r="V25"/>
       <c r="W25" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X25" s="5" t="n">
         <v>45299</v>
@@ -2795,7 +2793,7 @@
       </c>
       <c r="V26"/>
       <c r="W26" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X26" s="5" t="n">
         <v>45299</v>
@@ -2860,7 +2858,7 @@
       </c>
       <c r="V27"/>
       <c r="W27" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X27" s="5" t="n">
         <v>45299</v>
@@ -2923,7 +2921,7 @@
       </c>
       <c r="V28"/>
       <c r="W28" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X28" s="5" t="n">
         <v>45299</v>
@@ -2984,11 +2982,11 @@
         <v>45299</v>
       </c>
       <c r="U29" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="V29"/>
       <c r="W29" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X29" s="5" t="n">
         <v>45299</v>
@@ -3053,7 +3051,7 @@
       </c>
       <c r="V30"/>
       <c r="W30" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X30" s="5" t="n">
         <v>45299</v>
@@ -3118,7 +3116,7 @@
       </c>
       <c r="V31"/>
       <c r="W31" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X31" s="5" t="n">
         <v>45299</v>
@@ -3183,7 +3181,7 @@
       </c>
       <c r="V32"/>
       <c r="W32" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X32" s="5" t="n">
         <v>45299</v>
@@ -3246,7 +3244,7 @@
       </c>
       <c r="V33"/>
       <c r="W33" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X33" s="5" t="n">
         <v>45299</v>
@@ -3311,7 +3309,7 @@
       </c>
       <c r="V34"/>
       <c r="W34" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X34" s="5" t="n">
         <v>45299</v>
@@ -3376,7 +3374,7 @@
       </c>
       <c r="V35"/>
       <c r="W35" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X35" s="5" t="n">
         <v>45299</v>
@@ -3441,7 +3439,7 @@
       </c>
       <c r="V36"/>
       <c r="W36" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X36" s="5" t="n">
         <v>45299</v>
@@ -3506,7 +3504,7 @@
       </c>
       <c r="V37"/>
       <c r="W37" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X37" s="5" t="n">
         <v>45299</v>
@@ -3567,7 +3565,7 @@
       </c>
       <c r="V38"/>
       <c r="W38" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X38" s="5" t="n">
         <v>45299</v>
@@ -3628,7 +3626,7 @@
       </c>
       <c r="V39"/>
       <c r="W39" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X39" s="5" t="n">
         <v>45299</v>
@@ -3689,7 +3687,7 @@
       </c>
       <c r="V40"/>
       <c r="W40" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X40" s="5" t="n">
         <v>45299</v>
@@ -3748,11 +3746,11 @@
         <v>45299</v>
       </c>
       <c r="U41" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="V41"/>
       <c r="W41" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X41" s="5" t="n">
         <v>45299</v>
@@ -3811,7 +3809,7 @@
       </c>
       <c r="V42"/>
       <c r="W42" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X42" s="5" t="n">
         <v>45299</v>
@@ -3870,7 +3868,7 @@
       </c>
       <c r="V43"/>
       <c r="W43" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X43" s="5" t="n">
         <v>45299</v>
@@ -3933,7 +3931,7 @@
       </c>
       <c r="V44"/>
       <c r="W44" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X44" s="5" t="n">
         <v>45299</v>
@@ -3996,7 +3994,7 @@
       </c>
       <c r="V45"/>
       <c r="W45" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X45" s="5" t="n">
         <v>45299</v>
@@ -4047,7 +4045,7 @@
       <c r="U46"/>
       <c r="V46"/>
       <c r="W46" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X46" s="5" t="n">
         <v>45299</v>
@@ -4108,7 +4106,7 @@
       </c>
       <c r="V47"/>
       <c r="W47" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X47" s="5" t="n">
         <v>45299</v>
@@ -4171,7 +4169,7 @@
       </c>
       <c r="V48"/>
       <c r="W48" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X48" s="5" t="n">
         <v>45299</v>
@@ -4230,7 +4228,7 @@
       </c>
       <c r="V49"/>
       <c r="W49" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X49" s="5" t="n">
         <v>45299</v>
@@ -4287,7 +4285,7 @@
         <v>283</v>
       </c>
       <c r="W50" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X50" s="5" t="n">
         <v>45299</v>
@@ -4350,7 +4348,7 @@
       </c>
       <c r="V51"/>
       <c r="W51" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X51" s="5" t="n">
         <v>45299</v>
@@ -4415,7 +4413,7 @@
         <v>283</v>
       </c>
       <c r="W52" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X52" s="5" t="n">
         <v>45299</v>
@@ -4474,7 +4472,7 @@
       </c>
       <c r="V53"/>
       <c r="W53" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X53" s="5" t="n">
         <v>45299</v>
@@ -4531,7 +4529,7 @@
       </c>
       <c r="V54"/>
       <c r="W54" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X54" s="5" t="n">
         <v>45299</v>
@@ -4592,7 +4590,7 @@
       </c>
       <c r="V55"/>
       <c r="W55" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X55" s="5" t="n">
         <v>45299</v>
@@ -4643,7 +4641,7 @@
       <c r="U56"/>
       <c r="V56"/>
       <c r="W56" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X56" s="5" t="n">
         <v>45299</v>
@@ -4706,7 +4704,7 @@
       </c>
       <c r="V57"/>
       <c r="W57" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X57" s="5" t="n">
         <v>45299</v>
@@ -4757,7 +4755,7 @@
       <c r="U58"/>
       <c r="V58"/>
       <c r="W58" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X58" s="5" t="n">
         <v>45299</v>
@@ -4814,7 +4812,7 @@
       </c>
       <c r="V59"/>
       <c r="W59" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X59" s="5" t="n">
         <v>45299</v>
@@ -4865,7 +4863,7 @@
       <c r="U60"/>
       <c r="V60"/>
       <c r="W60" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X60" s="5" t="n">
         <v>45299</v>
@@ -4916,7 +4914,7 @@
       <c r="U61"/>
       <c r="V61"/>
       <c r="W61" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X61" s="5" t="n">
         <v>45299</v>
@@ -4971,11 +4969,11 @@
         <v>45299</v>
       </c>
       <c r="U62" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="V62"/>
       <c r="W62" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X62" s="5" t="n">
         <v>45299</v>
@@ -5030,11 +5028,11 @@
         <v>45299</v>
       </c>
       <c r="U63" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="V63"/>
       <c r="W63" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X63" s="5" t="n">
         <v>45299</v>
@@ -5093,7 +5091,7 @@
       </c>
       <c r="V64"/>
       <c r="W64" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X64" s="5" t="n">
         <v>45299</v>
@@ -5152,7 +5150,7 @@
       </c>
       <c r="V65"/>
       <c r="W65" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X65" s="5" t="n">
         <v>45299</v>
@@ -5211,7 +5209,7 @@
       </c>
       <c r="V66"/>
       <c r="W66" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X66" s="5" t="n">
         <v>45299</v>
@@ -5266,7 +5264,7 @@
       </c>
       <c r="V67"/>
       <c r="W67" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X67" s="5" t="n">
         <v>45299</v>
@@ -5325,7 +5323,7 @@
       </c>
       <c r="V68"/>
       <c r="W68" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X68" s="5" t="n">
         <v>45299</v>
@@ -5384,7 +5382,7 @@
       </c>
       <c r="V69"/>
       <c r="W69" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X69" s="5" t="n">
         <v>45299</v>
@@ -5443,7 +5441,7 @@
       </c>
       <c r="V70"/>
       <c r="W70" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X70" s="5" t="n">
         <v>45299</v>
@@ -5504,7 +5502,7 @@
         <v>284</v>
       </c>
       <c r="W71" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X71" s="5" t="n">
         <v>45299</v>
@@ -5563,7 +5561,7 @@
       </c>
       <c r="V72"/>
       <c r="W72" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X72" s="5" t="n">
         <v>45299</v>
@@ -5622,7 +5620,7 @@
       </c>
       <c r="V73"/>
       <c r="W73" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X73" s="5" t="n">
         <v>45299</v>
@@ -5681,7 +5679,7 @@
       </c>
       <c r="V74"/>
       <c r="W74" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X74" s="5" t="n">
         <v>45299</v>
@@ -5740,7 +5738,7 @@
       </c>
       <c r="V75"/>
       <c r="W75" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X75" s="5" t="n">
         <v>45299</v>
@@ -5789,7 +5787,7 @@
       <c r="U76"/>
       <c r="V76"/>
       <c r="W76" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X76" s="5" t="n">
         <v>45299</v>
@@ -5848,7 +5846,7 @@
       </c>
       <c r="V77"/>
       <c r="W77" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X77" s="5" t="n">
         <v>45299</v>
@@ -5911,11 +5909,11 @@
         <v>45299</v>
       </c>
       <c r="U78" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="V78"/>
       <c r="W78" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X78" s="5" t="n">
         <v>45299</v>
@@ -5974,7 +5972,7 @@
       </c>
       <c r="V79"/>
       <c r="W79" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X79" s="5" t="n">
         <v>45299</v>
@@ -6037,7 +6035,7 @@
       </c>
       <c r="V80"/>
       <c r="W80" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X80" s="5" t="n">
         <v>45299</v>
@@ -6096,7 +6094,7 @@
       </c>
       <c r="V81"/>
       <c r="W81" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X81" s="5" t="n">
         <v>45299</v>
@@ -6159,7 +6157,7 @@
       </c>
       <c r="V82"/>
       <c r="W82" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X82" s="5" t="n">
         <v>45299</v>
@@ -6222,7 +6220,7 @@
       </c>
       <c r="V83"/>
       <c r="W83" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X83" s="5" t="n">
         <v>45299</v>
@@ -6285,7 +6283,7 @@
       </c>
       <c r="V84"/>
       <c r="W84" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X84" s="5" t="n">
         <v>45299</v>
@@ -6348,7 +6346,7 @@
       </c>
       <c r="V85"/>
       <c r="W85" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X85" s="5" t="n">
         <v>45299</v>
@@ -6411,7 +6409,7 @@
       </c>
       <c r="V86"/>
       <c r="W86" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X86" s="5" t="n">
         <v>45299</v>
@@ -6476,7 +6474,7 @@
       </c>
       <c r="V87"/>
       <c r="W87" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X87" s="5" t="n">
         <v>45299</v>
@@ -6541,7 +6539,7 @@
       </c>
       <c r="V88"/>
       <c r="W88" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X88" s="5" t="n">
         <v>45299</v>
@@ -6604,7 +6602,7 @@
       </c>
       <c r="V89"/>
       <c r="W89" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X89" s="5" t="n">
         <v>45299</v>
@@ -6667,7 +6665,7 @@
       </c>
       <c r="V90"/>
       <c r="W90" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X90" s="5" t="n">
         <v>45299</v>
@@ -6730,7 +6728,7 @@
       </c>
       <c r="V91"/>
       <c r="W91" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X91" s="5" t="n">
         <v>45299</v>
@@ -6793,7 +6791,7 @@
       </c>
       <c r="V92"/>
       <c r="W92" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="X92" s="5" t="n">
         <v>45299</v>

</xml_diff>

<commit_message>
updated Quantiles with latest exports 7-15-24 (WQ_Discrete re-exported 7/11/24)
</commit_message>
<xml_diff>
--- a/output/ScriptResults/Database_Thresholds.xlsx
+++ b/output/ScriptResults/Database_Thresholds.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
   <si>
     <t>Just a database ID. Retaining this in future correspondence will allow for the most efficient update, based on this single column.</t>
   </si>
@@ -939,6 +939,12 @@
   </si>
   <si>
     <t xml:space="preserve">Water Column - Fluorescent dissolved organic matter, FDOM not included in SEACAR data export tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated: 2024-07-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database_Thresholds.xlsx, Git Commit ID: 51214cf344547100c5a54d26465d79cec9558701</t>
   </si>
 </sst>
 </file>
@@ -979,14 +985,11 @@
       <sz val="16"/>
       <color rgb="FF2F5496"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
       <b/>
     </font>
     <font>
@@ -1373,7 +1376,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>154</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" ht="158.44999999999999" customHeight="1">
@@ -1553,7 +1556,7 @@
         <v>283</v>
       </c>
       <c r="X8" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y8" s="6"/>
     </row>
@@ -1607,20 +1610,20 @@
         <v>284</v>
       </c>
       <c r="T9" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U9" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V9"/>
       <c r="W9" t="s">
         <v>283</v>
       </c>
       <c r="X9" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y9" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="10">
@@ -1671,20 +1674,20 @@
         <v>284</v>
       </c>
       <c r="T10" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U10" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V10"/>
       <c r="W10" t="s">
         <v>283</v>
       </c>
       <c r="X10" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y10" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="11">
@@ -1743,7 +1746,7 @@
         <v>283</v>
       </c>
       <c r="X11" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y11" s="6" t="n">
         <v>45314</v>
@@ -1799,7 +1802,7 @@
         <v>283</v>
       </c>
       <c r="X12" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y12" s="6"/>
     </row>
@@ -1851,20 +1854,20 @@
         <v>284</v>
       </c>
       <c r="T13" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U13" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V13"/>
       <c r="W13" t="s">
         <v>283</v>
       </c>
       <c r="X13" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y13" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="14">
@@ -1913,20 +1916,20 @@
         <v>284</v>
       </c>
       <c r="T14" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U14" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V14"/>
       <c r="W14" t="s">
         <v>283</v>
       </c>
       <c r="X14" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y14" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="15">
@@ -1971,7 +1974,7 @@
         <v>284</v>
       </c>
       <c r="T15" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U15"/>
       <c r="V15" t="s">
@@ -1981,10 +1984,10 @@
         <v>283</v>
       </c>
       <c r="X15" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y15" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="16">
@@ -2035,20 +2038,20 @@
         <v>284</v>
       </c>
       <c r="T16" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U16" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V16"/>
       <c r="W16" t="s">
         <v>283</v>
       </c>
       <c r="X16" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y16" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="17">
@@ -2097,7 +2100,7 @@
         <v>284</v>
       </c>
       <c r="T17" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U17"/>
       <c r="V17" t="s">
@@ -2107,10 +2110,10 @@
         <v>283</v>
       </c>
       <c r="X17" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y17" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="18">
@@ -2163,7 +2166,7 @@
         <v>283</v>
       </c>
       <c r="X18" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y18" s="6" t="n">
         <v>45257</v>
@@ -2217,20 +2220,20 @@
         <v>284</v>
       </c>
       <c r="T19" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U19" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V19"/>
       <c r="W19" t="s">
         <v>283</v>
       </c>
       <c r="X19" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y19" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="20">
@@ -2281,20 +2284,20 @@
         <v>284</v>
       </c>
       <c r="T20" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U20" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V20"/>
       <c r="W20" t="s">
         <v>283</v>
       </c>
       <c r="X20" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y20" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="21">
@@ -2345,20 +2348,20 @@
         <v>284</v>
       </c>
       <c r="T21" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U21" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V21"/>
       <c r="W21" t="s">
         <v>283</v>
       </c>
       <c r="X21" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y21" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="22">
@@ -2409,20 +2412,20 @@
         <v>284</v>
       </c>
       <c r="T22" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U22" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V22"/>
       <c r="W22" t="s">
         <v>283</v>
       </c>
       <c r="X22" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y22" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="23">
@@ -2475,20 +2478,20 @@
         <v>284</v>
       </c>
       <c r="T23" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U23" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V23"/>
       <c r="W23" t="s">
         <v>283</v>
       </c>
       <c r="X23" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y23" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="24">
@@ -2541,20 +2544,20 @@
         <v>284</v>
       </c>
       <c r="T24" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U24" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V24"/>
       <c r="W24" t="s">
         <v>283</v>
       </c>
       <c r="X24" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y24" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="25">
@@ -2607,7 +2610,7 @@
         <v>283</v>
       </c>
       <c r="X25" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y25" s="6"/>
     </row>
@@ -2659,20 +2662,20 @@
         <v>284</v>
       </c>
       <c r="T26" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U26" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V26"/>
       <c r="W26" t="s">
         <v>283</v>
       </c>
       <c r="X26" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y26" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="27">
@@ -2725,20 +2728,20 @@
         <v>284</v>
       </c>
       <c r="T27" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U27" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V27"/>
       <c r="W27" t="s">
         <v>283</v>
       </c>
       <c r="X27" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y27" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="28">
@@ -2793,20 +2796,20 @@
         <v>284</v>
       </c>
       <c r="T28" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U28" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V28"/>
       <c r="W28" t="s">
         <v>283</v>
       </c>
       <c r="X28" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y28" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="29">
@@ -2867,7 +2870,7 @@
         <v>283</v>
       </c>
       <c r="X29" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y29" s="6" t="n">
         <v>45314</v>
@@ -2925,20 +2928,20 @@
         <v>284</v>
       </c>
       <c r="T30" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U30" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V30"/>
       <c r="W30" t="s">
         <v>283</v>
       </c>
       <c r="X30" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y30" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="31">
@@ -2999,7 +3002,7 @@
         <v>283</v>
       </c>
       <c r="X31" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y31" s="6" t="n">
         <v>45314</v>
@@ -3055,20 +3058,20 @@
         <v>284</v>
       </c>
       <c r="T32" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U32" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V32"/>
       <c r="W32" t="s">
         <v>283</v>
       </c>
       <c r="X32" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y32" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="33">
@@ -3123,20 +3126,20 @@
         <v>284</v>
       </c>
       <c r="T33" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U33" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V33"/>
       <c r="W33" t="s">
         <v>283</v>
       </c>
       <c r="X33" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y33" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="34">
@@ -3197,7 +3200,7 @@
         <v>283</v>
       </c>
       <c r="X34" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y34" s="6" t="n">
         <v>45314</v>
@@ -3255,20 +3258,20 @@
         <v>284</v>
       </c>
       <c r="T35" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U35" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V35"/>
       <c r="W35" t="s">
         <v>283</v>
       </c>
       <c r="X35" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y35" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="36">
@@ -3329,7 +3332,7 @@
         <v>283</v>
       </c>
       <c r="X36" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y36" s="6" t="n">
         <v>45314</v>
@@ -3385,20 +3388,20 @@
         <v>284</v>
       </c>
       <c r="T37" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U37" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V37"/>
       <c r="W37" t="s">
         <v>283</v>
       </c>
       <c r="X37" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y37" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="38">
@@ -3453,20 +3456,20 @@
         <v>284</v>
       </c>
       <c r="T38" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U38" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V38"/>
       <c r="W38" t="s">
         <v>283</v>
       </c>
       <c r="X38" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y38" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="39">
@@ -3527,7 +3530,7 @@
         <v>283</v>
       </c>
       <c r="X39" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y39" s="6" t="n">
         <v>45314</v>
@@ -3585,20 +3588,20 @@
         <v>284</v>
       </c>
       <c r="T40" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U40" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V40"/>
       <c r="W40" t="s">
         <v>283</v>
       </c>
       <c r="X40" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y40" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="41">
@@ -3659,7 +3662,7 @@
         <v>283</v>
       </c>
       <c r="X41" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y41" s="6" t="n">
         <v>45314</v>
@@ -3713,20 +3716,20 @@
         <v>284</v>
       </c>
       <c r="T42" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U42" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V42"/>
       <c r="W42" t="s">
         <v>283</v>
       </c>
       <c r="X42" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y42" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="43">
@@ -3777,20 +3780,20 @@
         <v>284</v>
       </c>
       <c r="T43" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U43" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V43"/>
       <c r="W43" t="s">
         <v>283</v>
       </c>
       <c r="X43" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y43" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="44">
@@ -3841,20 +3844,20 @@
         <v>284</v>
       </c>
       <c r="T44" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U44" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V44"/>
       <c r="W44" t="s">
         <v>283</v>
       </c>
       <c r="X44" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y44" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="45">
@@ -3907,20 +3910,20 @@
         <v>284</v>
       </c>
       <c r="T45" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U45" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V45"/>
       <c r="W45" t="s">
         <v>283</v>
       </c>
       <c r="X45" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y45" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="46">
@@ -3979,7 +3982,7 @@
         <v>283</v>
       </c>
       <c r="X46" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y46" s="6"/>
     </row>
@@ -4033,20 +4036,20 @@
         <v>284</v>
       </c>
       <c r="T47" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U47" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V47"/>
       <c r="W47" t="s">
         <v>283</v>
       </c>
       <c r="X47" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y47" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="48">
@@ -4099,20 +4102,20 @@
         <v>284</v>
       </c>
       <c r="T48" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U48" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V48"/>
       <c r="W48" t="s">
         <v>283</v>
       </c>
       <c r="X48" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y48" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="49">
@@ -4171,7 +4174,7 @@
         <v>283</v>
       </c>
       <c r="X49" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y49" s="6" t="n">
         <v>45314</v>
@@ -4227,7 +4230,7 @@
         <v>283</v>
       </c>
       <c r="X50" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y50" s="6"/>
     </row>
@@ -4275,7 +4278,7 @@
         <v>284</v>
       </c>
       <c r="T51" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U51"/>
       <c r="V51" t="s">
@@ -4285,10 +4288,10 @@
         <v>283</v>
       </c>
       <c r="X51" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y51" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="52">
@@ -4337,7 +4340,7 @@
         <v>284</v>
       </c>
       <c r="T52" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U52"/>
       <c r="V52" t="s">
@@ -4347,10 +4350,10 @@
         <v>283</v>
       </c>
       <c r="X52" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y52" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="53">
@@ -4403,20 +4406,20 @@
         <v>284</v>
       </c>
       <c r="T53" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U53" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V53"/>
       <c r="W53" t="s">
         <v>283</v>
       </c>
       <c r="X53" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y53" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="54">
@@ -4467,10 +4470,10 @@
         <v>284</v>
       </c>
       <c r="T54" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U54" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V54" t="s">
         <v>296</v>
@@ -4479,10 +4482,10 @@
         <v>283</v>
       </c>
       <c r="X54" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y54" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="55">
@@ -4535,20 +4538,20 @@
         <v>284</v>
       </c>
       <c r="T55" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U55" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V55"/>
       <c r="W55" t="s">
         <v>283</v>
       </c>
       <c r="X55" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y55" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="56">
@@ -4601,10 +4604,10 @@
         <v>284</v>
       </c>
       <c r="T56" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U56" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V56" t="s">
         <v>296</v>
@@ -4613,10 +4616,10 @@
         <v>283</v>
       </c>
       <c r="X56" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y56" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="57">
@@ -4665,7 +4668,7 @@
         <v>284</v>
       </c>
       <c r="T57" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U57"/>
       <c r="V57" t="s">
@@ -4675,10 +4678,10 @@
         <v>283</v>
       </c>
       <c r="X57" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y57" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="58">
@@ -4733,7 +4736,7 @@
         <v>283</v>
       </c>
       <c r="X58" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y58" s="6" t="n">
         <v>45314</v>
@@ -4787,20 +4790,20 @@
         <v>284</v>
       </c>
       <c r="T59" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U59" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V59"/>
       <c r="W59" t="s">
         <v>283</v>
       </c>
       <c r="X59" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y59" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="60">
@@ -4853,7 +4856,7 @@
         <v>283</v>
       </c>
       <c r="X60" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y60" s="6"/>
     </row>
@@ -4903,7 +4906,7 @@
         <v>284</v>
       </c>
       <c r="T61" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U61"/>
       <c r="V61" t="s">
@@ -4913,10 +4916,10 @@
         <v>283</v>
       </c>
       <c r="X61" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y61" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="62">
@@ -4969,7 +4972,7 @@
         <v>283</v>
       </c>
       <c r="X62" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y62" s="6"/>
     </row>
@@ -5021,20 +5024,20 @@
         <v>284</v>
       </c>
       <c r="T63" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U63" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V63"/>
       <c r="W63" t="s">
         <v>283</v>
       </c>
       <c r="X63" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y63" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="64">
@@ -5087,7 +5090,7 @@
         <v>283</v>
       </c>
       <c r="X64" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y64" s="6"/>
     </row>
@@ -5141,7 +5144,7 @@
         <v>283</v>
       </c>
       <c r="X65" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y65" s="6"/>
     </row>
@@ -5191,20 +5194,20 @@
         <v>284</v>
       </c>
       <c r="T66" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U66" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V66"/>
       <c r="W66" t="s">
         <v>283</v>
       </c>
       <c r="X66" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y66" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="67">
@@ -5253,20 +5256,20 @@
         <v>284</v>
       </c>
       <c r="T67" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U67" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V67"/>
       <c r="W67" t="s">
         <v>283</v>
       </c>
       <c r="X67" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y67" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="68">
@@ -5303,7 +5306,7 @@
         <v>-0.0023</v>
       </c>
       <c r="O68" t="n">
-        <v>3.13939</v>
+        <v>3.139395</v>
       </c>
       <c r="P68" t="n">
         <v>0</v>
@@ -5315,20 +5318,20 @@
         <v>284</v>
       </c>
       <c r="T68" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U68" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V68"/>
       <c r="W68" t="s">
         <v>283</v>
       </c>
       <c r="X68" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y68" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="69">
@@ -5377,20 +5380,20 @@
         <v>284</v>
       </c>
       <c r="T69" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U69" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V69"/>
       <c r="W69" t="s">
         <v>283</v>
       </c>
       <c r="X69" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y69" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="70">
@@ -5439,20 +5442,20 @@
         <v>284</v>
       </c>
       <c r="T70" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U70" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V70"/>
       <c r="W70" t="s">
         <v>283</v>
       </c>
       <c r="X70" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y70" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="71">
@@ -5507,7 +5510,7 @@
         <v>283</v>
       </c>
       <c r="X71" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y71" s="6"/>
     </row>
@@ -5557,20 +5560,20 @@
         <v>284</v>
       </c>
       <c r="T72" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U72" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V72"/>
       <c r="W72" t="s">
         <v>283</v>
       </c>
       <c r="X72" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y72" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="73">
@@ -5619,20 +5622,20 @@
         <v>284</v>
       </c>
       <c r="T73" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U73" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V73"/>
       <c r="W73" t="s">
         <v>283</v>
       </c>
       <c r="X73" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y73" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="74">
@@ -5681,20 +5684,20 @@
         <v>284</v>
       </c>
       <c r="T74" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U74" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V74"/>
       <c r="W74" t="s">
         <v>283</v>
       </c>
       <c r="X74" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y74" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="75">
@@ -5743,10 +5746,10 @@
         <v>284</v>
       </c>
       <c r="T75" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U75" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V75" t="s">
         <v>304</v>
@@ -5755,10 +5758,10 @@
         <v>283</v>
       </c>
       <c r="X75" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y75" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="76">
@@ -5807,20 +5810,20 @@
         <v>284</v>
       </c>
       <c r="T76" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U76" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V76"/>
       <c r="W76" t="s">
         <v>283</v>
       </c>
       <c r="X76" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y76" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="77">
@@ -5869,20 +5872,20 @@
         <v>284</v>
       </c>
       <c r="T77" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U77" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V77"/>
       <c r="W77" t="s">
         <v>283</v>
       </c>
       <c r="X77" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y77" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="78">
@@ -5931,20 +5934,20 @@
         <v>284</v>
       </c>
       <c r="T78" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U78" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V78"/>
       <c r="W78" t="s">
         <v>283</v>
       </c>
       <c r="X78" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y78" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="79">
@@ -5993,20 +5996,20 @@
         <v>284</v>
       </c>
       <c r="T79" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U79" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V79"/>
       <c r="W79" t="s">
         <v>283</v>
       </c>
       <c r="X79" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y79" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="80">
@@ -6057,7 +6060,7 @@
         <v>283</v>
       </c>
       <c r="X80" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y80" s="6"/>
     </row>
@@ -6107,20 +6110,20 @@
         <v>284</v>
       </c>
       <c r="T81" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U81" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V81"/>
       <c r="W81" t="s">
         <v>283</v>
       </c>
       <c r="X81" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y81" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="82">
@@ -6177,20 +6180,20 @@
         <v>284</v>
       </c>
       <c r="T82" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U82" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V82"/>
       <c r="W82" t="s">
         <v>283</v>
       </c>
       <c r="X82" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y82" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="83">
@@ -6239,20 +6242,20 @@
         <v>284</v>
       </c>
       <c r="T83" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U83" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V83"/>
       <c r="W83" t="s">
         <v>283</v>
       </c>
       <c r="X83" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y83" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="84">
@@ -6305,20 +6308,20 @@
         <v>284</v>
       </c>
       <c r="T84" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U84" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V84"/>
       <c r="W84" t="s">
         <v>283</v>
       </c>
       <c r="X84" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y84" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="85">
@@ -6367,20 +6370,20 @@
         <v>284</v>
       </c>
       <c r="T85" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U85" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V85"/>
       <c r="W85" t="s">
         <v>283</v>
       </c>
       <c r="X85" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y85" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="86">
@@ -6439,7 +6442,7 @@
         <v>283</v>
       </c>
       <c r="X86" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y86" s="6" t="n">
         <v>45257</v>
@@ -6495,20 +6498,20 @@
         <v>284</v>
       </c>
       <c r="T87" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U87" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V87"/>
       <c r="W87" t="s">
         <v>283</v>
       </c>
       <c r="X87" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y87" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="88">
@@ -6561,20 +6564,20 @@
         <v>284</v>
       </c>
       <c r="T88" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U88" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V88"/>
       <c r="W88" t="s">
         <v>283</v>
       </c>
       <c r="X88" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y88" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="89">
@@ -6627,20 +6630,20 @@
         <v>284</v>
       </c>
       <c r="T89" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U89" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V89"/>
       <c r="W89" t="s">
         <v>283</v>
       </c>
       <c r="X89" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y89" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="90">
@@ -6693,20 +6696,20 @@
         <v>284</v>
       </c>
       <c r="T90" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U90" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V90"/>
       <c r="W90" t="s">
         <v>283</v>
       </c>
       <c r="X90" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y90" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="91">
@@ -6761,20 +6764,20 @@
         <v>284</v>
       </c>
       <c r="T91" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U91" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V91"/>
       <c r="W91" t="s">
         <v>283</v>
       </c>
       <c r="X91" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y91" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="92">
@@ -6829,20 +6832,20 @@
         <v>284</v>
       </c>
       <c r="T92" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U92" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V92"/>
       <c r="W92" t="s">
         <v>283</v>
       </c>
       <c r="X92" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y92" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="93">
@@ -6895,20 +6898,20 @@
         <v>284</v>
       </c>
       <c r="T93" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U93" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V93"/>
       <c r="W93" t="s">
         <v>283</v>
       </c>
       <c r="X93" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y93" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="94">
@@ -6961,20 +6964,20 @@
         <v>284</v>
       </c>
       <c r="T94" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U94" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V94"/>
       <c r="W94" t="s">
         <v>283</v>
       </c>
       <c r="X94" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y94" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="95">
@@ -7033,7 +7036,7 @@
         <v>283</v>
       </c>
       <c r="X95" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y95" s="6" t="n">
         <v>45257</v>
@@ -7089,20 +7092,20 @@
         <v>284</v>
       </c>
       <c r="T96" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="U96" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="V96"/>
       <c r="W96" t="s">
         <v>283</v>
       </c>
       <c r="X96" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="Y96" s="6" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Thresholds and Quantiles, 09-04-24 Combined Tables
</commit_message>
<xml_diff>
--- a/output/ScriptResults/Database_Thresholds.xlsx
+++ b/output/ScriptResults/Database_Thresholds.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
   <si>
     <t>Parameter Units.</t>
   </si>
@@ -987,6 +987,15 @@
   </si>
   <si>
     <t xml:space="preserve">Water Column - Fluorescent dissolved organic matter, FDOM not included in SEACAR data export tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated: 2024-09-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQ_Report_Render.R, Git Commit ID: 4613a4a191f05e3e604adbbffe6225f17403b427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database_Thresholds.xlsx, Git Commit ID: 4613a4a191f05e3e604adbbffe6225f17403b427</t>
   </si>
 </sst>
 </file>
@@ -1421,7 +1430,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>170</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" ht="158.44999999999999" customHeight="1">
@@ -1598,10 +1607,10 @@
         <v>298</v>
       </c>
       <c r="W8" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X8" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y8" s="7"/>
     </row>
@@ -1651,21 +1660,17 @@
       <c r="Q9" t="n">
         <v>0</v>
       </c>
-      <c r="S9" t="s">
-        <v>300</v>
-      </c>
-      <c r="T9" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S9"/>
+      <c r="T9" s="7"/>
       <c r="U9" t="s">
         <v>301</v>
       </c>
       <c r="V9" s="6"/>
       <c r="W9" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X9" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y9" s="7" t="n">
         <v>45517</v>
@@ -1715,21 +1720,17 @@
       <c r="Q10" t="n">
         <v>0</v>
       </c>
-      <c r="S10" t="s">
-        <v>300</v>
-      </c>
-      <c r="T10" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S10"/>
+      <c r="T10" s="7"/>
       <c r="U10" t="s">
         <v>301</v>
       </c>
       <c r="V10" s="6"/>
       <c r="W10" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X10" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y10" s="7" t="n">
         <v>45517</v>
@@ -1788,10 +1789,10 @@
       </c>
       <c r="V11" s="6"/>
       <c r="W11" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X11" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y11" s="7" t="n">
         <v>45314</v>
@@ -1844,10 +1845,10 @@
         <v>303</v>
       </c>
       <c r="W12" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X12" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y12" s="7"/>
     </row>
@@ -1895,21 +1896,17 @@
       <c r="Q13" t="n">
         <v>0</v>
       </c>
-      <c r="S13" t="s">
-        <v>300</v>
-      </c>
-      <c r="T13" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S13"/>
+      <c r="T13" s="7"/>
       <c r="U13" t="s">
         <v>301</v>
       </c>
       <c r="V13" s="6"/>
       <c r="W13" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X13" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y13" s="7" t="n">
         <v>45517</v>
@@ -1957,21 +1954,17 @@
       <c r="Q14" t="n">
         <v>0</v>
       </c>
-      <c r="S14" t="s">
-        <v>300</v>
-      </c>
-      <c r="T14" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S14"/>
+      <c r="T14" s="7"/>
       <c r="U14" t="s">
         <v>301</v>
       </c>
       <c r="V14" s="6"/>
       <c r="W14" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X14" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y14" s="7" t="n">
         <v>45517</v>
@@ -2015,21 +2008,17 @@
       <c r="Q15" t="n">
         <v>0</v>
       </c>
-      <c r="S15" t="s">
-        <v>300</v>
-      </c>
-      <c r="T15" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S15"/>
+      <c r="T15" s="7"/>
       <c r="U15"/>
       <c r="V15" s="6" t="s">
         <v>304</v>
       </c>
       <c r="W15" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X15" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y15" s="7" t="n">
         <v>45517</v>
@@ -2079,21 +2068,17 @@
       <c r="Q16" t="n">
         <v>0</v>
       </c>
-      <c r="S16" t="s">
-        <v>300</v>
-      </c>
-      <c r="T16" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S16"/>
+      <c r="T16" s="7"/>
       <c r="U16" t="s">
         <v>301</v>
       </c>
       <c r="V16" s="6"/>
       <c r="W16" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X16" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y16" s="7" t="n">
         <v>45517</v>
@@ -2141,21 +2126,17 @@
       <c r="Q17" t="n">
         <v>0</v>
       </c>
-      <c r="S17" t="s">
-        <v>300</v>
-      </c>
-      <c r="T17" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S17"/>
+      <c r="T17" s="7"/>
       <c r="U17"/>
       <c r="V17" s="6" t="s">
         <v>304</v>
       </c>
       <c r="W17" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X17" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y17" s="7" t="n">
         <v>45517</v>
@@ -2208,10 +2189,10 @@
         <v>306</v>
       </c>
       <c r="W18" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X18" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y18" s="7" t="n">
         <v>45257</v>
@@ -2261,21 +2242,17 @@
       <c r="Q19" t="n">
         <v>0</v>
       </c>
-      <c r="S19" t="s">
-        <v>300</v>
-      </c>
-      <c r="T19" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S19"/>
+      <c r="T19" s="7"/>
       <c r="U19" t="s">
         <v>301</v>
       </c>
       <c r="V19" s="6"/>
       <c r="W19" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X19" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y19" s="7" t="n">
         <v>45517</v>
@@ -2325,21 +2302,17 @@
       <c r="Q20" t="n">
         <v>0</v>
       </c>
-      <c r="S20" t="s">
-        <v>300</v>
-      </c>
-      <c r="T20" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S20"/>
+      <c r="T20" s="7"/>
       <c r="U20" t="s">
         <v>301</v>
       </c>
       <c r="V20" s="6"/>
       <c r="W20" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X20" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y20" s="7" t="n">
         <v>45517</v>
@@ -2389,21 +2362,17 @@
       <c r="Q21" t="n">
         <v>0</v>
       </c>
-      <c r="S21" t="s">
-        <v>300</v>
-      </c>
-      <c r="T21" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S21"/>
+      <c r="T21" s="7"/>
       <c r="U21" t="s">
         <v>301</v>
       </c>
       <c r="V21" s="6"/>
       <c r="W21" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X21" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y21" s="7" t="n">
         <v>45517</v>
@@ -2453,21 +2422,17 @@
       <c r="Q22" t="n">
         <v>0</v>
       </c>
-      <c r="S22" t="s">
-        <v>300</v>
-      </c>
-      <c r="T22" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S22"/>
+      <c r="T22" s="7"/>
       <c r="U22" t="s">
         <v>301</v>
       </c>
       <c r="V22" s="6"/>
       <c r="W22" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X22" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y22" s="7" t="n">
         <v>45517</v>
@@ -2519,21 +2484,17 @@
       <c r="Q23" t="n">
         <v>0</v>
       </c>
-      <c r="S23" t="s">
-        <v>300</v>
-      </c>
-      <c r="T23" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S23"/>
+      <c r="T23" s="7"/>
       <c r="U23" t="s">
         <v>301</v>
       </c>
       <c r="V23" s="6"/>
       <c r="W23" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X23" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y23" s="7" t="n">
         <v>45517</v>
@@ -2585,21 +2546,17 @@
       <c r="Q24" t="n">
         <v>0</v>
       </c>
-      <c r="S24" t="s">
-        <v>300</v>
-      </c>
-      <c r="T24" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S24"/>
+      <c r="T24" s="7"/>
       <c r="U24" t="s">
         <v>301</v>
       </c>
       <c r="V24" s="6"/>
       <c r="W24" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X24" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y24" s="7" t="n">
         <v>45517</v>
@@ -2652,10 +2609,10 @@
         <v>307</v>
       </c>
       <c r="W25" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X25" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y25" s="7"/>
     </row>
@@ -2703,21 +2660,17 @@
       <c r="Q26" t="n">
         <v>0</v>
       </c>
-      <c r="S26" t="s">
-        <v>300</v>
-      </c>
-      <c r="T26" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S26"/>
+      <c r="T26" s="7"/>
       <c r="U26" t="s">
         <v>301</v>
       </c>
       <c r="V26" s="6"/>
       <c r="W26" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X26" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y26" s="7" t="n">
         <v>45517</v>
@@ -2772,10 +2725,10 @@
       </c>
       <c r="V27" s="6"/>
       <c r="W27" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X27" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y27" s="7" t="n">
         <v>45314</v>
@@ -2829,21 +2782,17 @@
       <c r="Q28" t="n">
         <v>0</v>
       </c>
-      <c r="S28" t="s">
-        <v>300</v>
-      </c>
-      <c r="T28" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S28"/>
+      <c r="T28" s="7"/>
       <c r="U28" t="s">
         <v>301</v>
       </c>
       <c r="V28" s="6"/>
       <c r="W28" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X28" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y28" s="7" t="n">
         <v>45517</v>
@@ -2904,10 +2853,10 @@
       </c>
       <c r="V29" s="6"/>
       <c r="W29" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X29" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y29" s="7" t="n">
         <v>45314</v>
@@ -2961,21 +2910,17 @@
       <c r="Q30" t="n">
         <v>0</v>
       </c>
-      <c r="S30" t="s">
-        <v>300</v>
-      </c>
-      <c r="T30" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S30"/>
+      <c r="T30" s="7"/>
       <c r="U30" t="s">
         <v>301</v>
       </c>
       <c r="V30" s="6"/>
       <c r="W30" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X30" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y30" s="7" t="n">
         <v>45517</v>
@@ -3029,21 +2974,17 @@
       <c r="Q31" t="n">
         <v>0</v>
       </c>
-      <c r="S31" t="s">
-        <v>300</v>
-      </c>
-      <c r="T31" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S31"/>
+      <c r="T31" s="7"/>
       <c r="U31" t="s">
         <v>301</v>
       </c>
       <c r="V31" s="6"/>
       <c r="W31" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X31" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y31" s="7" t="n">
         <v>45517</v>
@@ -3098,10 +3039,10 @@
       </c>
       <c r="V32" s="6"/>
       <c r="W32" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X32" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y32" s="7" t="n">
         <v>45314</v>
@@ -3155,21 +3096,17 @@
       <c r="Q33" t="n">
         <v>0</v>
       </c>
-      <c r="S33" t="s">
-        <v>300</v>
-      </c>
-      <c r="T33" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S33"/>
+      <c r="T33" s="7"/>
       <c r="U33" t="s">
         <v>301</v>
       </c>
       <c r="V33" s="6"/>
       <c r="W33" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X33" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y33" s="7" t="n">
         <v>45517</v>
@@ -3230,10 +3167,10 @@
       </c>
       <c r="V34" s="6"/>
       <c r="W34" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X34" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y34" s="7" t="n">
         <v>45314</v>
@@ -3287,21 +3224,17 @@
       <c r="Q35" t="n">
         <v>0</v>
       </c>
-      <c r="S35" t="s">
-        <v>300</v>
-      </c>
-      <c r="T35" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S35"/>
+      <c r="T35" s="7"/>
       <c r="U35" t="s">
         <v>301</v>
       </c>
       <c r="V35" s="6"/>
       <c r="W35" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X35" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y35" s="7" t="n">
         <v>45517</v>
@@ -3355,21 +3288,17 @@
       <c r="Q36" t="n">
         <v>0</v>
       </c>
-      <c r="S36" t="s">
-        <v>300</v>
-      </c>
-      <c r="T36" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S36"/>
+      <c r="T36" s="7"/>
       <c r="U36" t="s">
         <v>301</v>
       </c>
       <c r="V36" s="6"/>
       <c r="W36" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X36" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y36" s="7" t="n">
         <v>45517</v>
@@ -3424,10 +3353,10 @@
       </c>
       <c r="V37" s="6"/>
       <c r="W37" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X37" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y37" s="7" t="n">
         <v>45314</v>
@@ -3481,21 +3410,17 @@
       <c r="Q38" t="n">
         <v>0</v>
       </c>
-      <c r="S38" t="s">
-        <v>300</v>
-      </c>
-      <c r="T38" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S38"/>
+      <c r="T38" s="7"/>
       <c r="U38" t="s">
         <v>301</v>
       </c>
       <c r="V38" s="6"/>
       <c r="W38" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X38" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y38" s="7" t="n">
         <v>45517</v>
@@ -3556,10 +3481,10 @@
       </c>
       <c r="V39" s="6"/>
       <c r="W39" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X39" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y39" s="7" t="n">
         <v>45314</v>
@@ -3613,21 +3538,17 @@
       <c r="Q40" t="n">
         <v>0</v>
       </c>
-      <c r="S40" t="s">
-        <v>300</v>
-      </c>
-      <c r="T40" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S40"/>
+      <c r="T40" s="7"/>
       <c r="U40" t="s">
         <v>301</v>
       </c>
       <c r="V40" s="6"/>
       <c r="W40" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X40" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y40" s="7" t="n">
         <v>45517</v>
@@ -3681,21 +3602,17 @@
       <c r="Q41" t="n">
         <v>0</v>
       </c>
-      <c r="S41" t="s">
-        <v>300</v>
-      </c>
-      <c r="T41" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S41"/>
+      <c r="T41" s="7"/>
       <c r="U41" t="s">
         <v>301</v>
       </c>
       <c r="V41" s="6"/>
       <c r="W41" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X41" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y41" s="7" t="n">
         <v>45517</v>
@@ -3745,21 +3662,17 @@
       <c r="Q42" t="n">
         <v>0</v>
       </c>
-      <c r="S42" t="s">
-        <v>300</v>
-      </c>
-      <c r="T42" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S42"/>
+      <c r="T42" s="7"/>
       <c r="U42" t="s">
         <v>301</v>
       </c>
       <c r="V42" s="6"/>
       <c r="W42" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X42" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y42" s="7" t="n">
         <v>45517</v>
@@ -3809,21 +3722,17 @@
       <c r="Q43" t="n">
         <v>0</v>
       </c>
-      <c r="S43" t="s">
-        <v>300</v>
-      </c>
-      <c r="T43" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S43"/>
+      <c r="T43" s="7"/>
       <c r="U43" t="s">
         <v>301</v>
       </c>
       <c r="V43" s="6"/>
       <c r="W43" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X43" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y43" s="7" t="n">
         <v>45517</v>
@@ -3873,21 +3782,17 @@
       <c r="Q44" t="n">
         <v>0</v>
       </c>
-      <c r="S44" t="s">
-        <v>300</v>
-      </c>
-      <c r="T44" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S44"/>
+      <c r="T44" s="7"/>
       <c r="U44" t="s">
         <v>301</v>
       </c>
       <c r="V44" s="6"/>
       <c r="W44" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X44" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y44" s="7" t="n">
         <v>45517</v>
@@ -3939,21 +3844,17 @@
       <c r="Q45" t="n">
         <v>0</v>
       </c>
-      <c r="S45" t="s">
-        <v>300</v>
-      </c>
-      <c r="T45" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S45"/>
+      <c r="T45" s="7"/>
       <c r="U45" t="s">
         <v>301</v>
       </c>
       <c r="V45" s="6"/>
       <c r="W45" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X45" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y45" s="7" t="n">
         <v>45517</v>
@@ -4012,10 +3913,10 @@
       </c>
       <c r="V46" s="6"/>
       <c r="W46" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X46" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y46" s="7"/>
     </row>
@@ -4065,21 +3966,17 @@
       <c r="Q47" t="n">
         <v>0</v>
       </c>
-      <c r="S47" t="s">
-        <v>300</v>
-      </c>
-      <c r="T47" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S47"/>
+      <c r="T47" s="7"/>
       <c r="U47" t="s">
         <v>301</v>
       </c>
       <c r="V47" s="6"/>
       <c r="W47" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X47" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y47" s="7" t="n">
         <v>45517</v>
@@ -4131,21 +4028,17 @@
       <c r="Q48" t="n">
         <v>0</v>
       </c>
-      <c r="S48" t="s">
-        <v>300</v>
-      </c>
-      <c r="T48" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S48"/>
+      <c r="T48" s="7"/>
       <c r="U48" t="s">
         <v>301</v>
       </c>
       <c r="V48" s="6"/>
       <c r="W48" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X48" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y48" s="7" t="n">
         <v>45517</v>
@@ -4204,10 +4097,10 @@
       </c>
       <c r="V49" s="6"/>
       <c r="W49" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X49" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y49" s="7" t="n">
         <v>45314</v>
@@ -4260,10 +4153,10 @@
         <v>309</v>
       </c>
       <c r="W50" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X50" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y50" s="7"/>
     </row>
@@ -4307,21 +4200,17 @@
       <c r="Q51" t="n">
         <v>0</v>
       </c>
-      <c r="S51" t="s">
-        <v>300</v>
-      </c>
-      <c r="T51" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S51"/>
+      <c r="T51" s="7"/>
       <c r="U51"/>
       <c r="V51" s="6" t="s">
         <v>310</v>
       </c>
       <c r="W51" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X51" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y51" s="7" t="n">
         <v>45517</v>
@@ -4369,21 +4258,17 @@
       <c r="Q52" t="n">
         <v>0</v>
       </c>
-      <c r="S52" t="s">
-        <v>300</v>
-      </c>
-      <c r="T52" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S52"/>
+      <c r="T52" s="7"/>
       <c r="U52"/>
       <c r="V52" s="6" t="s">
         <v>311</v>
       </c>
       <c r="W52" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X52" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y52" s="7" t="n">
         <v>45517</v>
@@ -4435,21 +4320,17 @@
       <c r="Q53" t="n">
         <v>0</v>
       </c>
-      <c r="S53" t="s">
-        <v>300</v>
-      </c>
-      <c r="T53" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S53"/>
+      <c r="T53" s="7"/>
       <c r="U53" t="s">
         <v>301</v>
       </c>
       <c r="V53" s="6"/>
       <c r="W53" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X53" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y53" s="7" t="n">
         <v>45517</v>
@@ -4499,12 +4380,8 @@
       <c r="Q54" t="n">
         <v>1</v>
       </c>
-      <c r="S54" t="s">
-        <v>300</v>
-      </c>
-      <c r="T54" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S54"/>
+      <c r="T54" s="7"/>
       <c r="U54" t="s">
         <v>301</v>
       </c>
@@ -4512,10 +4389,10 @@
         <v>312</v>
       </c>
       <c r="W54" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X54" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y54" s="7" t="n">
         <v>45517</v>
@@ -4567,21 +4444,17 @@
       <c r="Q55" t="n">
         <v>0</v>
       </c>
-      <c r="S55" t="s">
-        <v>300</v>
-      </c>
-      <c r="T55" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S55"/>
+      <c r="T55" s="7"/>
       <c r="U55" t="s">
         <v>301</v>
       </c>
       <c r="V55" s="6"/>
       <c r="W55" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X55" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y55" s="7" t="n">
         <v>45517</v>
@@ -4633,12 +4506,8 @@
       <c r="Q56" t="n">
         <v>1</v>
       </c>
-      <c r="S56" t="s">
-        <v>300</v>
-      </c>
-      <c r="T56" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S56"/>
+      <c r="T56" s="7"/>
       <c r="U56" t="s">
         <v>301</v>
       </c>
@@ -4646,10 +4515,10 @@
         <v>312</v>
       </c>
       <c r="W56" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X56" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y56" s="7" t="n">
         <v>45517</v>
@@ -4697,21 +4566,17 @@
       <c r="Q57" t="n">
         <v>0</v>
       </c>
-      <c r="S57" t="s">
-        <v>300</v>
-      </c>
-      <c r="T57" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S57"/>
+      <c r="T57" s="7"/>
       <c r="U57"/>
       <c r="V57" s="6" t="s">
         <v>313</v>
       </c>
       <c r="W57" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X57" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y57" s="7" t="n">
         <v>45517</v>
@@ -4766,10 +4631,10 @@
         <v>314</v>
       </c>
       <c r="W58" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X58" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y58" s="7" t="n">
         <v>45314</v>
@@ -4819,21 +4684,17 @@
       <c r="Q59" t="n">
         <v>0</v>
       </c>
-      <c r="S59" t="s">
-        <v>300</v>
-      </c>
-      <c r="T59" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S59"/>
+      <c r="T59" s="7"/>
       <c r="U59" t="s">
         <v>301</v>
       </c>
       <c r="V59" s="6"/>
       <c r="W59" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X59" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y59" s="7" t="n">
         <v>45517</v>
@@ -4886,10 +4747,10 @@
         <v>315</v>
       </c>
       <c r="W60" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X60" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y60" s="7"/>
     </row>
@@ -4935,21 +4796,17 @@
       <c r="Q61" t="n">
         <v>0</v>
       </c>
-      <c r="S61" t="s">
-        <v>300</v>
-      </c>
-      <c r="T61" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S61"/>
+      <c r="T61" s="7"/>
       <c r="U61"/>
       <c r="V61" s="6" t="s">
         <v>316</v>
       </c>
       <c r="W61" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X61" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y61" s="7" t="n">
         <v>45517</v>
@@ -5002,10 +4859,10 @@
         <v>317</v>
       </c>
       <c r="W62" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X62" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y62" s="7"/>
     </row>
@@ -5053,21 +4910,17 @@
       <c r="Q63" t="n">
         <v>0</v>
       </c>
-      <c r="S63" t="s">
-        <v>300</v>
-      </c>
-      <c r="T63" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S63"/>
+      <c r="T63" s="7"/>
       <c r="U63" t="s">
         <v>301</v>
       </c>
       <c r="V63" s="6"/>
       <c r="W63" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X63" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y63" s="7" t="n">
         <v>45517</v>
@@ -5120,10 +4973,10 @@
         <v>318</v>
       </c>
       <c r="W64" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X64" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y64" s="7"/>
     </row>
@@ -5174,10 +5027,10 @@
         <v>319</v>
       </c>
       <c r="W65" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X65" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y65" s="7"/>
     </row>
@@ -5223,21 +5076,17 @@
       <c r="Q66" t="n">
         <v>0</v>
       </c>
-      <c r="S66" t="s">
-        <v>300</v>
-      </c>
-      <c r="T66" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S66"/>
+      <c r="T66" s="7"/>
       <c r="U66" t="s">
         <v>301</v>
       </c>
       <c r="V66" s="6"/>
       <c r="W66" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X66" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y66" s="7" t="n">
         <v>45517</v>
@@ -5274,10 +5123,10 @@
       <c r="L67"/>
       <c r="M67"/>
       <c r="N67" t="n">
-        <v>-0.025045</v>
+        <v>-0.0231</v>
       </c>
       <c r="O67" t="n">
-        <v>5.67755</v>
+        <v>5.0979</v>
       </c>
       <c r="P67" t="n">
         <v>0</v>
@@ -5289,20 +5138,20 @@
         <v>300</v>
       </c>
       <c r="T67" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U67" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V67" s="6"/>
       <c r="W67" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X67" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y67" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="68">
@@ -5336,10 +5185,10 @@
       <c r="L68"/>
       <c r="M68"/>
       <c r="N68" t="n">
-        <v>-0.0023</v>
+        <v>-0.002</v>
       </c>
       <c r="O68" t="n">
-        <v>3.139395</v>
+        <v>2.83719</v>
       </c>
       <c r="P68" t="n">
         <v>0</v>
@@ -5351,20 +5200,20 @@
         <v>300</v>
       </c>
       <c r="T68" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U68" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V68" s="6"/>
       <c r="W68" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X68" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y68" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="69">
@@ -5401,7 +5250,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O69" t="n">
-        <v>0.79552</v>
+        <v>0.95771</v>
       </c>
       <c r="P69" t="n">
         <v>0</v>
@@ -5413,20 +5262,20 @@
         <v>300</v>
       </c>
       <c r="T69" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U69" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V69" s="6"/>
       <c r="W69" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X69" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y69" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="70">
@@ -5460,10 +5309,10 @@
       <c r="L70"/>
       <c r="M70"/>
       <c r="N70" t="n">
-        <v>-0.000001</v>
+        <v>0.00014</v>
       </c>
       <c r="O70" t="n">
-        <v>0.08</v>
+        <v>0.3</v>
       </c>
       <c r="P70" t="n">
         <v>0</v>
@@ -5475,20 +5324,20 @@
         <v>300</v>
       </c>
       <c r="T70" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U70" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V70" s="6"/>
       <c r="W70" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X70" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y70" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="71">
@@ -5540,10 +5389,10 @@
       </c>
       <c r="V71" s="6"/>
       <c r="W71" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X71" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y71" s="7"/>
     </row>
@@ -5589,21 +5438,17 @@
       <c r="Q72" t="n">
         <v>0</v>
       </c>
-      <c r="S72" t="s">
-        <v>300</v>
-      </c>
-      <c r="T72" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S72"/>
+      <c r="T72" s="7"/>
       <c r="U72" t="s">
         <v>301</v>
       </c>
       <c r="V72" s="6"/>
       <c r="W72" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X72" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y72" s="7" t="n">
         <v>45517</v>
@@ -5640,10 +5485,10 @@
       <c r="L73"/>
       <c r="M73"/>
       <c r="N73" t="n">
-        <v>-0.000001</v>
+        <v>0.0001</v>
       </c>
       <c r="O73" t="n">
-        <v>5.07</v>
+        <v>4.81323</v>
       </c>
       <c r="P73" t="n">
         <v>0</v>
@@ -5655,20 +5500,20 @@
         <v>300</v>
       </c>
       <c r="T73" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U73" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V73" s="6"/>
       <c r="W73" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X73" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y73" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="74">
@@ -5705,7 +5550,7 @@
         <v>0.00007</v>
       </c>
       <c r="O74" t="n">
-        <v>4.2</v>
+        <v>4.12935</v>
       </c>
       <c r="P74" t="n">
         <v>0</v>
@@ -5717,20 +5562,20 @@
         <v>300</v>
       </c>
       <c r="T74" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U74" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V74" s="6"/>
       <c r="W74" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X74" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y74" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="75">
@@ -5767,7 +5612,7 @@
         <v>0.00006</v>
       </c>
       <c r="O75" t="n">
-        <v>2.7462</v>
+        <v>2.77562</v>
       </c>
       <c r="P75" t="n">
         <v>1</v>
@@ -5779,22 +5624,22 @@
         <v>300</v>
       </c>
       <c r="T75" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U75" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V75" s="6" t="s">
         <v>320</v>
       </c>
       <c r="W75" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X75" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y75" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="76">
@@ -5831,7 +5676,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O76" t="n">
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
       <c r="P76" t="n">
         <v>0</v>
@@ -5843,20 +5688,20 @@
         <v>300</v>
       </c>
       <c r="T76" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U76" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V76" s="6"/>
       <c r="W76" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X76" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y76" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="77">
@@ -5893,7 +5738,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O77" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="P77" t="n">
         <v>0</v>
@@ -5905,20 +5750,20 @@
         <v>300</v>
       </c>
       <c r="T77" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U77" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V77" s="6"/>
       <c r="W77" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X77" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y77" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="78">
@@ -5955,7 +5800,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O78" t="n">
-        <v>116.508</v>
+        <v>111.0856</v>
       </c>
       <c r="P78" t="n">
         <v>0</v>
@@ -5967,20 +5812,20 @@
         <v>300</v>
       </c>
       <c r="T78" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U78" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V78" s="6"/>
       <c r="W78" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X78" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y78" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="79">
@@ -6017,7 +5862,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O79" t="n">
-        <v>711.61</v>
+        <v>699.3698</v>
       </c>
       <c r="P79" t="n">
         <v>0</v>
@@ -6029,20 +5874,20 @@
         <v>300</v>
       </c>
       <c r="T79" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U79" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V79" s="6"/>
       <c r="W79" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X79" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y79" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="80">
@@ -6090,10 +5935,10 @@
         <v>321</v>
       </c>
       <c r="W80" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X80" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y80" s="7"/>
     </row>
@@ -6139,21 +5984,17 @@
       <c r="Q81" t="n">
         <v>0</v>
       </c>
-      <c r="S81" t="s">
-        <v>300</v>
-      </c>
-      <c r="T81" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S81"/>
+      <c r="T81" s="7"/>
       <c r="U81" t="s">
         <v>301</v>
       </c>
       <c r="V81" s="6"/>
       <c r="W81" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X81" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y81" s="7" t="n">
         <v>45517</v>
@@ -6201,7 +6042,7 @@
         <v>0.1</v>
       </c>
       <c r="O82" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="P82" t="n">
         <v>0</v>
@@ -6213,20 +6054,20 @@
         <v>300</v>
       </c>
       <c r="T82" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U82" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V82" s="6"/>
       <c r="W82" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X82" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y82" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="83">
@@ -6263,7 +6104,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O83" t="n">
-        <v>180.854</v>
+        <v>177</v>
       </c>
       <c r="P83" t="n">
         <v>0</v>
@@ -6275,20 +6116,20 @@
         <v>300</v>
       </c>
       <c r="T83" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U83" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V83" s="6"/>
       <c r="W83" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X83" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y83" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="84">
@@ -6329,7 +6170,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O84" t="n">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="P84" t="n">
         <v>0</v>
@@ -6341,20 +6182,20 @@
         <v>300</v>
       </c>
       <c r="T84" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U84" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V84" s="6"/>
       <c r="W84" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X84" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y84" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="85">
@@ -6391,7 +6232,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O85" t="n">
-        <v>124.736197</v>
+        <v>126</v>
       </c>
       <c r="P85" t="n">
         <v>0</v>
@@ -6403,20 +6244,20 @@
         <v>300</v>
       </c>
       <c r="T85" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U85" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V85" s="6"/>
       <c r="W85" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X85" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y85" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="86">
@@ -6472,10 +6313,10 @@
       </c>
       <c r="V86" s="6"/>
       <c r="W86" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X86" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y86" s="7" t="n">
         <v>45257</v>
@@ -6507,16 +6348,16 @@
         <v>250</v>
       </c>
       <c r="I87" t="n">
-        <v>0.000001</v>
+        <v>-0.000001</v>
       </c>
       <c r="J87" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K87"/>
       <c r="L87"/>
       <c r="M87"/>
       <c r="N87" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="O87" t="n">
         <v>14</v>
@@ -6531,20 +6372,20 @@
         <v>300</v>
       </c>
       <c r="T87" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U87" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V87" s="6"/>
       <c r="W87" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X87" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y87" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="88">
@@ -6585,7 +6426,7 @@
         <v>1.6</v>
       </c>
       <c r="O88" t="n">
-        <v>170.8</v>
+        <v>170.52318</v>
       </c>
       <c r="P88" t="n">
         <v>0</v>
@@ -6597,20 +6438,20 @@
         <v>300</v>
       </c>
       <c r="T88" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U88" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V88" s="6"/>
       <c r="W88" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X88" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y88" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="89">
@@ -6639,7 +6480,7 @@
         <v>195</v>
       </c>
       <c r="I89" t="n">
-        <v>0.000001</v>
+        <v>-0.000001</v>
       </c>
       <c r="J89" t="n">
         <v>310</v>
@@ -6648,10 +6489,10 @@
       <c r="L89"/>
       <c r="M89"/>
       <c r="N89" t="n">
-        <v>0.313613</v>
+        <v>0.342931</v>
       </c>
       <c r="O89" t="n">
-        <v>175.291124</v>
+        <v>174.98932</v>
       </c>
       <c r="P89" t="n">
         <v>0</v>
@@ -6663,20 +6504,20 @@
         <v>300</v>
       </c>
       <c r="T89" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U89" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V89" s="6"/>
       <c r="W89" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X89" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y89" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="90">
@@ -6725,21 +6566,17 @@
       <c r="Q90" t="n">
         <v>0</v>
       </c>
-      <c r="S90" t="s">
-        <v>300</v>
-      </c>
-      <c r="T90" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S90"/>
+      <c r="T90" s="7"/>
       <c r="U90" t="s">
         <v>301</v>
       </c>
       <c r="V90" s="6"/>
       <c r="W90" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X90" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y90" s="7" t="n">
         <v>45517</v>
@@ -6785,7 +6622,7 @@
         <v>-0.000001</v>
       </c>
       <c r="O91" t="n">
-        <v>41</v>
+        <v>41.1</v>
       </c>
       <c r="P91" t="n">
         <v>0</v>
@@ -6797,20 +6634,20 @@
         <v>300</v>
       </c>
       <c r="T91" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U91" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V91" s="6"/>
       <c r="W91" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X91" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y91" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="92">
@@ -6853,7 +6690,7 @@
         <v>0.0054</v>
       </c>
       <c r="O92" t="n">
-        <v>60.381584</v>
+        <v>60.71</v>
       </c>
       <c r="P92" t="n">
         <v>0</v>
@@ -6865,20 +6702,20 @@
         <v>300</v>
       </c>
       <c r="T92" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U92" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V92" s="6"/>
       <c r="W92" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X92" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y92" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="93">
@@ -6927,21 +6764,17 @@
       <c r="Q93" t="n">
         <v>0</v>
       </c>
-      <c r="S93" t="s">
-        <v>300</v>
-      </c>
-      <c r="T93" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S93"/>
+      <c r="T93" s="7"/>
       <c r="U93" t="s">
         <v>301</v>
       </c>
       <c r="V93" s="6"/>
       <c r="W93" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X93" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y93" s="7" t="n">
         <v>45517</v>
@@ -6982,7 +6815,7 @@
       <c r="L94"/>
       <c r="M94"/>
       <c r="N94" t="n">
-        <v>6.59466</v>
+        <v>6.6</v>
       </c>
       <c r="O94" t="n">
         <v>33.9</v>
@@ -6997,20 +6830,20 @@
         <v>300</v>
       </c>
       <c r="T94" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="U94" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="V94" s="6"/>
       <c r="W94" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X94" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y94" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
     </row>
     <row r="95">
@@ -7066,10 +6899,10 @@
       </c>
       <c r="V95" s="6"/>
       <c r="W95" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X95" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y95" s="7" t="n">
         <v>45257</v>
@@ -7121,21 +6954,17 @@
       <c r="Q96" t="n">
         <v>0</v>
       </c>
-      <c r="S96" t="s">
-        <v>300</v>
-      </c>
-      <c r="T96" s="7" t="n">
-        <v>45517</v>
-      </c>
+      <c r="S96"/>
+      <c r="T96" s="7"/>
       <c r="U96" t="s">
         <v>301</v>
       </c>
       <c r="V96" s="6"/>
       <c r="W96" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="X96" s="7" t="n">
-        <v>45517</v>
+        <v>45547</v>
       </c>
       <c r="Y96" s="7" t="n">
         <v>45517</v>

</xml_diff>

<commit_message>
update db_thresholds; add files_used.txt
</commit_message>
<xml_diff>
--- a/output/ScriptResults/Database_Thresholds.xlsx
+++ b/output/ScriptResults/Database_Thresholds.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="326">
   <si>
     <t>Parameter Units.</t>
   </si>
@@ -989,13 +989,16 @@
     <t xml:space="preserve">Water Column - Fluorescent dissolved organic matter, FDOM not included in SEACAR data export tables</t>
   </si>
   <si>
-    <t xml:space="preserve">Updated: 2024-09-12</t>
+    <t xml:space="preserve">Script Run: 2024-11-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">IQ_Report_Render.R, Git Commit ID: 4613a4a191f05e3e604adbbffe6225f17403b427</t>
   </si>
   <si>
-    <t xml:space="preserve">Database_Thresholds.xlsx, Git Commit ID: 4613a4a191f05e3e604adbbffe6225f17403b427</t>
+    <t xml:space="preserve">Database_Thresholds.xlsx, Git Commit ID: 00a27356deb3dd3ebc41bb112fe7b3bfe3e44544</t>
   </si>
 </sst>
 </file>
@@ -1428,9 +1431,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>322</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" ht="158.44999999999999" customHeight="1">
@@ -1607,10 +1615,10 @@
         <v>298</v>
       </c>
       <c r="W8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X8" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y8" s="7"/>
     </row>
@@ -1667,10 +1675,10 @@
       </c>
       <c r="V9" s="6"/>
       <c r="W9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X9" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y9" s="7" t="n">
         <v>45517</v>
@@ -1727,10 +1735,10 @@
       </c>
       <c r="V10" s="6"/>
       <c r="W10" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X10" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y10" s="7" t="n">
         <v>45517</v>
@@ -1789,10 +1797,10 @@
       </c>
       <c r="V11" s="6"/>
       <c r="W11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X11" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y11" s="7" t="n">
         <v>45314</v>
@@ -1845,10 +1853,10 @@
         <v>303</v>
       </c>
       <c r="W12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X12" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y12" s="7"/>
     </row>
@@ -1903,10 +1911,10 @@
       </c>
       <c r="V13" s="6"/>
       <c r="W13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X13" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y13" s="7" t="n">
         <v>45517</v>
@@ -1961,10 +1969,10 @@
       </c>
       <c r="V14" s="6"/>
       <c r="W14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X14" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y14" s="7" t="n">
         <v>45517</v>
@@ -2015,10 +2023,10 @@
         <v>304</v>
       </c>
       <c r="W15" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X15" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y15" s="7" t="n">
         <v>45517</v>
@@ -2075,10 +2083,10 @@
       </c>
       <c r="V16" s="6"/>
       <c r="W16" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X16" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y16" s="7" t="n">
         <v>45517</v>
@@ -2133,10 +2141,10 @@
         <v>304</v>
       </c>
       <c r="W17" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X17" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y17" s="7" t="n">
         <v>45517</v>
@@ -2189,10 +2197,10 @@
         <v>306</v>
       </c>
       <c r="W18" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X18" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y18" s="7" t="n">
         <v>45257</v>
@@ -2249,10 +2257,10 @@
       </c>
       <c r="V19" s="6"/>
       <c r="W19" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X19" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y19" s="7" t="n">
         <v>45517</v>
@@ -2309,10 +2317,10 @@
       </c>
       <c r="V20" s="6"/>
       <c r="W20" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X20" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y20" s="7" t="n">
         <v>45517</v>
@@ -2369,10 +2377,10 @@
       </c>
       <c r="V21" s="6"/>
       <c r="W21" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X21" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y21" s="7" t="n">
         <v>45517</v>
@@ -2429,10 +2437,10 @@
       </c>
       <c r="V22" s="6"/>
       <c r="W22" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X22" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y22" s="7" t="n">
         <v>45517</v>
@@ -2491,10 +2499,10 @@
       </c>
       <c r="V23" s="6"/>
       <c r="W23" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X23" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y23" s="7" t="n">
         <v>45517</v>
@@ -2553,10 +2561,10 @@
       </c>
       <c r="V24" s="6"/>
       <c r="W24" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X24" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y24" s="7" t="n">
         <v>45517</v>
@@ -2609,10 +2617,10 @@
         <v>307</v>
       </c>
       <c r="W25" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X25" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y25" s="7"/>
     </row>
@@ -2667,10 +2675,10 @@
       </c>
       <c r="V26" s="6"/>
       <c r="W26" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X26" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y26" s="7" t="n">
         <v>45517</v>
@@ -2725,10 +2733,10 @@
       </c>
       <c r="V27" s="6"/>
       <c r="W27" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X27" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y27" s="7" t="n">
         <v>45314</v>
@@ -2789,10 +2797,10 @@
       </c>
       <c r="V28" s="6"/>
       <c r="W28" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X28" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y28" s="7" t="n">
         <v>45517</v>
@@ -2853,10 +2861,10 @@
       </c>
       <c r="V29" s="6"/>
       <c r="W29" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X29" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y29" s="7" t="n">
         <v>45314</v>
@@ -2917,10 +2925,10 @@
       </c>
       <c r="V30" s="6"/>
       <c r="W30" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X30" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y30" s="7" t="n">
         <v>45517</v>
@@ -2981,10 +2989,10 @@
       </c>
       <c r="V31" s="6"/>
       <c r="W31" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X31" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y31" s="7" t="n">
         <v>45517</v>
@@ -3039,10 +3047,10 @@
       </c>
       <c r="V32" s="6"/>
       <c r="W32" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X32" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y32" s="7" t="n">
         <v>45314</v>
@@ -3103,10 +3111,10 @@
       </c>
       <c r="V33" s="6"/>
       <c r="W33" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X33" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y33" s="7" t="n">
         <v>45517</v>
@@ -3167,10 +3175,10 @@
       </c>
       <c r="V34" s="6"/>
       <c r="W34" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X34" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y34" s="7" t="n">
         <v>45314</v>
@@ -3231,10 +3239,10 @@
       </c>
       <c r="V35" s="6"/>
       <c r="W35" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X35" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y35" s="7" t="n">
         <v>45517</v>
@@ -3295,10 +3303,10 @@
       </c>
       <c r="V36" s="6"/>
       <c r="W36" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X36" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y36" s="7" t="n">
         <v>45517</v>
@@ -3353,10 +3361,10 @@
       </c>
       <c r="V37" s="6"/>
       <c r="W37" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X37" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y37" s="7" t="n">
         <v>45314</v>
@@ -3417,10 +3425,10 @@
       </c>
       <c r="V38" s="6"/>
       <c r="W38" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X38" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y38" s="7" t="n">
         <v>45517</v>
@@ -3481,10 +3489,10 @@
       </c>
       <c r="V39" s="6"/>
       <c r="W39" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X39" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y39" s="7" t="n">
         <v>45314</v>
@@ -3545,10 +3553,10 @@
       </c>
       <c r="V40" s="6"/>
       <c r="W40" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X40" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y40" s="7" t="n">
         <v>45517</v>
@@ -3609,10 +3617,10 @@
       </c>
       <c r="V41" s="6"/>
       <c r="W41" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X41" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y41" s="7" t="n">
         <v>45517</v>
@@ -3669,10 +3677,10 @@
       </c>
       <c r="V42" s="6"/>
       <c r="W42" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X42" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y42" s="7" t="n">
         <v>45517</v>
@@ -3729,10 +3737,10 @@
       </c>
       <c r="V43" s="6"/>
       <c r="W43" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X43" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y43" s="7" t="n">
         <v>45517</v>
@@ -3789,10 +3797,10 @@
       </c>
       <c r="V44" s="6"/>
       <c r="W44" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X44" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y44" s="7" t="n">
         <v>45517</v>
@@ -3851,10 +3859,10 @@
       </c>
       <c r="V45" s="6"/>
       <c r="W45" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X45" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y45" s="7" t="n">
         <v>45517</v>
@@ -3913,10 +3921,10 @@
       </c>
       <c r="V46" s="6"/>
       <c r="W46" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X46" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y46" s="7"/>
     </row>
@@ -3973,10 +3981,10 @@
       </c>
       <c r="V47" s="6"/>
       <c r="W47" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X47" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y47" s="7" t="n">
         <v>45517</v>
@@ -4035,10 +4043,10 @@
       </c>
       <c r="V48" s="6"/>
       <c r="W48" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X48" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y48" s="7" t="n">
         <v>45517</v>
@@ -4097,10 +4105,10 @@
       </c>
       <c r="V49" s="6"/>
       <c r="W49" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X49" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y49" s="7" t="n">
         <v>45314</v>
@@ -4153,10 +4161,10 @@
         <v>309</v>
       </c>
       <c r="W50" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X50" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y50" s="7"/>
     </row>
@@ -4207,10 +4215,10 @@
         <v>310</v>
       </c>
       <c r="W51" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X51" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y51" s="7" t="n">
         <v>45517</v>
@@ -4265,10 +4273,10 @@
         <v>311</v>
       </c>
       <c r="W52" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X52" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y52" s="7" t="n">
         <v>45517</v>
@@ -4327,10 +4335,10 @@
       </c>
       <c r="V53" s="6"/>
       <c r="W53" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X53" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y53" s="7" t="n">
         <v>45517</v>
@@ -4389,10 +4397,10 @@
         <v>312</v>
       </c>
       <c r="W54" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X54" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y54" s="7" t="n">
         <v>45517</v>
@@ -4451,10 +4459,10 @@
       </c>
       <c r="V55" s="6"/>
       <c r="W55" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X55" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y55" s="7" t="n">
         <v>45517</v>
@@ -4515,10 +4523,10 @@
         <v>312</v>
       </c>
       <c r="W56" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X56" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y56" s="7" t="n">
         <v>45517</v>
@@ -4573,10 +4581,10 @@
         <v>313</v>
       </c>
       <c r="W57" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X57" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y57" s="7" t="n">
         <v>45517</v>
@@ -4631,10 +4639,10 @@
         <v>314</v>
       </c>
       <c r="W58" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X58" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y58" s="7" t="n">
         <v>45314</v>
@@ -4691,10 +4699,10 @@
       </c>
       <c r="V59" s="6"/>
       <c r="W59" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X59" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y59" s="7" t="n">
         <v>45517</v>
@@ -4747,10 +4755,10 @@
         <v>315</v>
       </c>
       <c r="W60" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X60" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y60" s="7"/>
     </row>
@@ -4803,10 +4811,10 @@
         <v>316</v>
       </c>
       <c r="W61" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X61" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y61" s="7" t="n">
         <v>45517</v>
@@ -4859,10 +4867,10 @@
         <v>317</v>
       </c>
       <c r="W62" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X62" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y62" s="7"/>
     </row>
@@ -4917,10 +4925,10 @@
       </c>
       <c r="V63" s="6"/>
       <c r="W63" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X63" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y63" s="7" t="n">
         <v>45517</v>
@@ -4973,10 +4981,10 @@
         <v>318</v>
       </c>
       <c r="W64" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X64" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y64" s="7"/>
     </row>
@@ -5027,10 +5035,10 @@
         <v>319</v>
       </c>
       <c r="W65" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X65" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y65" s="7"/>
     </row>
@@ -5083,10 +5091,10 @@
       </c>
       <c r="V66" s="6"/>
       <c r="W66" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X66" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y66" s="7" t="n">
         <v>45517</v>
@@ -5138,20 +5146,20 @@
         <v>300</v>
       </c>
       <c r="T67" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U67" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V67" s="6"/>
       <c r="W67" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X67" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y67" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="68">
@@ -5188,7 +5196,7 @@
         <v>-0.002</v>
       </c>
       <c r="O68" t="n">
-        <v>2.83719</v>
+        <v>2.837179</v>
       </c>
       <c r="P68" t="n">
         <v>0</v>
@@ -5200,20 +5208,20 @@
         <v>300</v>
       </c>
       <c r="T68" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U68" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V68" s="6"/>
       <c r="W68" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X68" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y68" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="69">
@@ -5262,20 +5270,20 @@
         <v>300</v>
       </c>
       <c r="T69" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U69" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V69" s="6"/>
       <c r="W69" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X69" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y69" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="70">
@@ -5324,20 +5332,20 @@
         <v>300</v>
       </c>
       <c r="T70" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U70" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V70" s="6"/>
       <c r="W70" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X70" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y70" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="71">
@@ -5389,10 +5397,10 @@
       </c>
       <c r="V71" s="6"/>
       <c r="W71" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X71" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y71" s="7"/>
     </row>
@@ -5445,10 +5453,10 @@
       </c>
       <c r="V72" s="6"/>
       <c r="W72" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X72" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y72" s="7" t="n">
         <v>45517</v>
@@ -5500,20 +5508,20 @@
         <v>300</v>
       </c>
       <c r="T73" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U73" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V73" s="6"/>
       <c r="W73" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X73" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y73" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="74">
@@ -5562,20 +5570,20 @@
         <v>300</v>
       </c>
       <c r="T74" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U74" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V74" s="6"/>
       <c r="W74" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X74" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y74" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="75">
@@ -5624,22 +5632,22 @@
         <v>300</v>
       </c>
       <c r="T75" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U75" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V75" s="6" t="s">
         <v>320</v>
       </c>
       <c r="W75" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X75" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y75" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="76">
@@ -5688,20 +5696,20 @@
         <v>300</v>
       </c>
       <c r="T76" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U76" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V76" s="6"/>
       <c r="W76" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X76" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y76" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="77">
@@ -5750,20 +5758,20 @@
         <v>300</v>
       </c>
       <c r="T77" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U77" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V77" s="6"/>
       <c r="W77" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X77" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y77" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="78">
@@ -5812,20 +5820,20 @@
         <v>300</v>
       </c>
       <c r="T78" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U78" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V78" s="6"/>
       <c r="W78" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X78" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y78" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="79">
@@ -5874,20 +5882,20 @@
         <v>300</v>
       </c>
       <c r="T79" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U79" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V79" s="6"/>
       <c r="W79" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X79" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y79" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="80">
@@ -5935,10 +5943,10 @@
         <v>321</v>
       </c>
       <c r="W80" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X80" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y80" s="7"/>
     </row>
@@ -5991,10 +5999,10 @@
       </c>
       <c r="V81" s="6"/>
       <c r="W81" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X81" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y81" s="7" t="n">
         <v>45517</v>
@@ -6054,20 +6062,20 @@
         <v>300</v>
       </c>
       <c r="T82" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U82" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V82" s="6"/>
       <c r="W82" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X82" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y82" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="83">
@@ -6116,20 +6124,20 @@
         <v>300</v>
       </c>
       <c r="T83" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U83" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V83" s="6"/>
       <c r="W83" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X83" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y83" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="84">
@@ -6182,20 +6190,20 @@
         <v>300</v>
       </c>
       <c r="T84" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U84" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V84" s="6"/>
       <c r="W84" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X84" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y84" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="85">
@@ -6244,20 +6252,20 @@
         <v>300</v>
       </c>
       <c r="T85" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U85" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V85" s="6"/>
       <c r="W85" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X85" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y85" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="86">
@@ -6313,10 +6321,10 @@
       </c>
       <c r="V86" s="6"/>
       <c r="W86" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X86" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y86" s="7" t="n">
         <v>45257</v>
@@ -6351,7 +6359,7 @@
         <v>-0.000001</v>
       </c>
       <c r="J87" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="K87"/>
       <c r="L87"/>
@@ -6372,20 +6380,20 @@
         <v>300</v>
       </c>
       <c r="T87" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U87" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V87" s="6"/>
       <c r="W87" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X87" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y87" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="88">
@@ -6438,20 +6446,20 @@
         <v>300</v>
       </c>
       <c r="T88" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U88" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V88" s="6"/>
       <c r="W88" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X88" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y88" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="89">
@@ -6504,20 +6512,20 @@
         <v>300</v>
       </c>
       <c r="T89" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U89" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V89" s="6"/>
       <c r="W89" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X89" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y89" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="90">
@@ -6573,10 +6581,10 @@
       </c>
       <c r="V90" s="6"/>
       <c r="W90" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X90" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y90" s="7" t="n">
         <v>45517</v>
@@ -6634,20 +6642,20 @@
         <v>300</v>
       </c>
       <c r="T91" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U91" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V91" s="6"/>
       <c r="W91" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X91" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y91" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="92">
@@ -6702,20 +6710,20 @@
         <v>300</v>
       </c>
       <c r="T92" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U92" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V92" s="6"/>
       <c r="W92" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X92" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y92" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="93">
@@ -6771,10 +6779,10 @@
       </c>
       <c r="V93" s="6"/>
       <c r="W93" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X93" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y93" s="7" t="n">
         <v>45517</v>
@@ -6830,20 +6838,20 @@
         <v>300</v>
       </c>
       <c r="T94" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="U94" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="V94" s="6"/>
       <c r="W94" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X94" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y94" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="95">
@@ -6899,10 +6907,10 @@
       </c>
       <c r="V95" s="6"/>
       <c r="W95" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X95" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y95" s="7" t="n">
         <v>45257</v>
@@ -6961,10 +6969,10 @@
       </c>
       <c r="V96" s="6"/>
       <c r="W96" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X96" s="7" t="n">
-        <v>45547</v>
+        <v>45621</v>
       </c>
       <c r="Y96" s="7" t="n">
         <v>45517</v>

</xml_diff>